<commit_message>
Final update - minor changes to functions/comments
</commit_message>
<xml_diff>
--- a/Reports/ReportC-Top_5_Interests_by_Gender.xlsx
+++ b/Reports/ReportC-Top_5_Interests_by_Gender.xlsx
@@ -308,7 +308,7 @@
   <pageSetup paperSize="9" fitToWidth="1" fitToHeight="1" scale="100" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>Top 5 Interests By Gender</oddHeader>
-    <oddFooter>Produced on 22MAY2023 by james.wright.</oddFooter>
+    <oddFooter>Produced on 24MAY2023 by james.wright.</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -365,7 +365,7 @@
   <pageSetup paperSize="9" fitToWidth="1" fitToHeight="1" scale="100" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>Top 5 Interests By Gender</oddHeader>
-    <oddFooter>Produced on 22MAY2023 by james.wright.</oddFooter>
+    <oddFooter>Produced on 24MAY2023 by james.wright.</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>